<commit_message>
Fix U.S. ICD-9 switch date
</commit_message>
<xml_diff>
--- a/data/ucod/united_states/comparable_data_since_1959.xlsx
+++ b/data/ucod/united_states/comparable_data_since_1959.xlsx
@@ -2277,13 +2277,13 @@
         <v>1902106</v>
       </c>
       <c r="C20">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D20">
-        <v>49928</v>
+        <v>51232</v>
       </c>
       <c r="E20">
-        <v>2643</v>
+        <v>2972</v>
       </c>
       <c r="F20">
         <v>1687</v>
@@ -2298,10 +2298,10 @@
         <v>8525</v>
       </c>
       <c r="J20">
-        <v>53899</v>
+        <v>53906</v>
       </c>
       <c r="K20">
-        <v>385721</v>
+        <v>386990</v>
       </c>
       <c r="L20">
         <v>23427</v>
@@ -2310,7 +2310,7 @@
         <v>33024</v>
       </c>
       <c r="N20">
-        <v>49747</v>
+        <v>49740</v>
       </c>
       <c r="O20">
         <v>28758</v>
@@ -2322,7 +2322,7 @@
         <v>30879</v>
       </c>
       <c r="R20">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="S20">
         <v>16</v>
@@ -2340,7 +2340,7 @@
         <v>340</v>
       </c>
       <c r="X20">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="Y20">
         <v>196</v>
@@ -2349,7 +2349,7 @@
         <v>127</v>
       </c>
       <c r="AA20">
-        <v>5092</v>
+        <v>5698</v>
       </c>
       <c r="AB20">
         <v>22374</v>
@@ -2372,13 +2372,13 @@
         <v>1930627</v>
       </c>
       <c r="C21">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D21">
-        <v>54302</v>
+        <v>58355</v>
       </c>
       <c r="E21">
-        <v>2608</v>
+        <v>2919</v>
       </c>
       <c r="F21">
         <v>1718</v>
@@ -2393,10 +2393,10 @@
         <v>8878</v>
       </c>
       <c r="J21">
-        <v>53433</v>
+        <v>53438</v>
       </c>
       <c r="K21">
-        <v>395993</v>
+        <v>397323</v>
       </c>
       <c r="L21">
         <v>22055</v>
@@ -2405,7 +2405,7 @@
         <v>33878</v>
       </c>
       <c r="N21">
-        <v>52658</v>
+        <v>52653</v>
       </c>
       <c r="O21">
         <v>28951</v>
@@ -2417,7 +2417,7 @@
         <v>30105</v>
       </c>
       <c r="R21">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S21">
         <v>11</v>
@@ -2435,7 +2435,7 @@
         <v>403</v>
       </c>
       <c r="X21">
-        <v>54</v>
+        <v>13</v>
       </c>
       <c r="Y21">
         <v>169</v>
@@ -2444,7 +2444,7 @@
         <v>139</v>
       </c>
       <c r="AA21">
-        <v>4903</v>
+        <v>5493</v>
       </c>
       <c r="AB21">
         <v>21894</v>

</xml_diff>